<commit_message>
FoPITY file updates and add SYSHECF pumped hydro csv (US version)
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/IT/Initial Time.xlsx
+++ b/InputData/plcy-schd/IT/Initial Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\plcy-schd\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E56E08-3411-4295-8CF7-4C86D7D20CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6939DCCA-9404-4B78-B99D-019E0F4A0BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="3150" windowWidth="19245" windowHeight="11595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="26025" windowHeight="14265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>